<commit_message>
Implemented new calibration coefficients
</commit_message>
<xml_diff>
--- a/data/Calibration/Calibration_continents_20240527.xlsx
+++ b/data/Calibration/Calibration_continents_20240527.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoDMS\ProjDir\2BURP\data\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjDir\Jip\2BURP\data\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA5E77-0CCF-46E8-9C77-A77A9819F024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E96AE0-CCE5-443F-A4FE-C0C417CBE335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="21105" xr2:uid="{912D1024-3E9A-4235-8027-2E86B942876C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{912D1024-3E9A-4235-8027-2E86B942876C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calib_results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Africa</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Landslide_prone</t>
+  </si>
+  <si>
+    <t>Dependent</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1"/>
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fixes in definition of suitability
Updates to calibration generation and grid costs to reflect name change in countries/per_grid (now per_domain)

Field name change in Excel sheet (Australia & Oceania to Australia_Oceania)
</commit_message>
<xml_diff>
--- a/data/Calibration/Calibration_continents_20240527.xlsx
+++ b/data/Calibration/Calibration_continents_20240527.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjDir\Jip\2BURP\data\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjDir\2BURP\data\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E96AE0-CCE5-443F-A4FE-C0C417CBE335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A5AD6C-A9CF-4F62-8AB3-402F79DA16F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{912D1024-3E9A-4235-8027-2E86B942876C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{912D1024-3E9A-4235-8027-2E86B942876C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calib_results" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Asia</t>
   </si>
   <si>
-    <t>Australia &amp; Oceania</t>
-  </si>
-  <si>
     <t>ln_PopulationDensity_2000_8dir</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Dependent</t>
+  </si>
+  <si>
+    <t>Australia_Oceania</t>
   </si>
 </sst>
 </file>
@@ -152,7 +152,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -487,7 +487,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -512,7 +512,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>0.70199999999999996</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>-8.9999999999999993E-3</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>-1.0999999999999999E-2</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>-0.09</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>-0.25600000000000001</v>

</xml_diff>